<commit_message>
Continua con el Jason
</commit_message>
<xml_diff>
--- a/contenido/Filtro Gespro.xlsx
+++ b/contenido/Filtro Gespro.xlsx
@@ -20596,20 +20596,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:XEF117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C107" sqref="C107"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" style="24"/>
     <col min="2" max="2" width="17.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="48" style="12" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="22" style="24"/>
     <col min="5" max="5" width="5.6640625" style="32" customWidth="1"/>
     <col min="6" max="16384" width="22" style="1"/>
@@ -20630,7 +20629,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:16360" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16360" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
         <v>222</v>
       </c>
@@ -20639,7 +20638,7 @@
       <c r="D2" s="50"/>
       <c r="E2" s="51"/>
     </row>
-    <row r="3" spans="1:16360" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>181</v>
       </c>
@@ -20673,7 +20672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16360" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>174</v>
       </c>
@@ -20690,7 +20689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16360" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>180</v>
       </c>
@@ -20724,7 +20723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16360" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="41" t="s">
         <v>176</v>
       </c>
@@ -20741,7 +20740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16360" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="41" t="s">
         <v>176</v>
       </c>
@@ -20758,7 +20757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16360" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>172</v>
       </c>
@@ -20775,7 +20774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16360" s="8" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16360" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="43" t="s">
         <v>178</v>
       </c>
@@ -20792,7 +20791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16360" s="8" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16360" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="43" t="s">
         <v>178</v>
       </c>
@@ -20809,7 +20808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16360" s="8" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16360" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="43" t="s">
         <v>178</v>
       </c>
@@ -37181,7 +37180,7 @@
       <c r="XEE13" s="7"/>
       <c r="XEF13" s="7"/>
     </row>
-    <row r="14" spans="1:16360" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="36" t="s">
         <v>178</v>
       </c>
@@ -37198,7 +37197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16360" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16360" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
         <v>176</v>
       </c>
@@ -37215,7 +37214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16360" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16360" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="41" t="s">
         <v>176</v>
       </c>
@@ -37232,7 +37231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="41" t="s">
         <v>189</v>
       </c>
@@ -37249,7 +37248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="41" t="s">
         <v>173</v>
       </c>
@@ -37385,7 +37384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="41" t="s">
         <v>177</v>
       </c>
@@ -37402,7 +37401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="41" t="s">
         <v>174</v>
       </c>
@@ -37572,7 +37571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="41" t="s">
         <v>218</v>
       </c>
@@ -37589,7 +37588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="41" t="s">
         <v>180</v>
       </c>
@@ -37623,7 +37622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="36" t="s">
         <v>188</v>
       </c>
@@ -37657,7 +37656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>181</v>
       </c>
@@ -37674,7 +37673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="41" t="s">
         <v>181</v>
       </c>
@@ -37691,7 +37690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="41" t="s">
         <v>172</v>
       </c>
@@ -37708,7 +37707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="41" t="s">
         <v>173</v>
       </c>
@@ -37725,7 +37724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="41" t="s">
         <v>172</v>
       </c>
@@ -37742,7 +37741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="41" t="s">
         <v>176</v>
       </c>
@@ -37759,7 +37758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="41" t="s">
         <v>175</v>
       </c>
@@ -37793,7 +37792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="41" t="s">
         <v>181</v>
       </c>
@@ -37844,7 +37843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="41" t="s">
         <v>173</v>
       </c>
@@ -37861,7 +37860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="41" t="s">
         <v>176</v>
       </c>
@@ -37878,7 +37877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="41" t="s">
         <v>219</v>
       </c>
@@ -37895,7 +37894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="41" t="s">
         <v>219</v>
       </c>
@@ -37912,7 +37911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="41" t="s">
         <v>219</v>
       </c>
@@ -37929,7 +37928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="41" t="s">
         <v>219</v>
       </c>
@@ -37946,7 +37945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="41" t="s">
         <v>173</v>
       </c>
@@ -38065,7 +38064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="41" t="s">
         <v>178</v>
       </c>
@@ -38082,7 +38081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="41" t="s">
         <v>174</v>
       </c>
@@ -38099,7 +38098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="41" t="s">
         <v>180</v>
       </c>
@@ -38116,7 +38115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="41" t="s">
         <v>174</v>
       </c>
@@ -38133,7 +38132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="41" t="s">
         <v>176</v>
       </c>
@@ -38150,7 +38149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="41" t="s">
         <v>174</v>
       </c>
@@ -38167,7 +38166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="41" t="s">
         <v>174</v>
       </c>
@@ -38184,7 +38183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="41" t="s">
         <v>172</v>
       </c>
@@ -38201,7 +38200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="41" t="s">
         <v>176</v>
       </c>
@@ -38218,7 +38217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="41" t="s">
         <v>176</v>
       </c>
@@ -38235,7 +38234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="41" t="s">
         <v>172</v>
       </c>
@@ -38252,7 +38251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="41" t="s">
         <v>181</v>
       </c>
@@ -38269,7 +38268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="41" t="s">
         <v>178</v>
       </c>
@@ -38286,7 +38285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="41" t="s">
         <v>174</v>
       </c>
@@ -38303,7 +38302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="41" t="s">
         <v>176</v>
       </c>
@@ -38320,7 +38319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="41" t="s">
         <v>181</v>
       </c>
@@ -38337,7 +38336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="41" t="s">
         <v>28</v>
       </c>
@@ -38354,7 +38353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="41" t="s">
         <v>190</v>
       </c>
@@ -38371,7 +38370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="41" t="s">
         <v>181</v>
       </c>
@@ -38388,7 +38387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="41" t="s">
         <v>173</v>
       </c>
@@ -38405,7 +38404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="41" t="s">
         <v>173</v>
       </c>
@@ -38422,7 +38421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="41" t="s">
         <v>173</v>
       </c>
@@ -38439,7 +38438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="41" t="s">
         <v>173</v>
       </c>
@@ -38456,7 +38455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="41" t="s">
         <v>188</v>
       </c>
@@ -38473,7 +38472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="41" t="s">
         <v>173</v>
       </c>
@@ -38490,7 +38489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="41" t="s">
         <v>173</v>
       </c>
@@ -38507,7 +38506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="41" t="s">
         <v>173</v>
       </c>
@@ -38524,7 +38523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="41" t="s">
         <v>174</v>
       </c>
@@ -38541,7 +38540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="41" t="s">
         <v>178</v>
       </c>
@@ -38558,7 +38557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="36" t="s">
         <v>28</v>
       </c>
@@ -38575,7 +38574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="41" t="s">
         <v>28</v>
       </c>
@@ -38592,7 +38591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="41" t="s">
         <v>28</v>
       </c>
@@ -38609,7 +38608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="41" t="s">
         <v>174</v>
       </c>
@@ -38626,7 +38625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="36" t="s">
         <v>28</v>
       </c>
@@ -38643,7 +38642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="36" t="s">
         <v>181</v>
       </c>
@@ -38660,7 +38659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="36" t="s">
         <v>221</v>
       </c>
@@ -38677,7 +38676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="36" t="s">
         <v>178</v>
       </c>
@@ -38697,7 +38696,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="103" spans="1:6" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="36" t="s">
         <v>181</v>
       </c>
@@ -38714,7 +38713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="41" t="s">
         <v>218</v>
       </c>
@@ -38731,7 +38730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="36" t="s">
         <v>213</v>
       </c>
@@ -38748,7 +38747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:6" s="9" customFormat="1" ht="25.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="41" t="s">
         <v>178</v>
       </c>
@@ -38796,7 +38795,7 @@
     <row r="111" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E111" s="32">
         <f>SUBTOTAL(9,E3:E110)</f>
-        <v>29</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -38849,13 +38848,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:XEF106">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Otros"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:XEF106"/>
   <mergeCells count="1">
     <mergeCell ref="A2:E2"/>
   </mergeCells>

</xml_diff>

<commit_message>
Se incorporan 33 jason para la búsquedas de palabras
</commit_message>
<xml_diff>
--- a/contenido/Filtro Gespro.xlsx
+++ b/contenido/Filtro Gespro.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\ColeccionRecursosGespro\contenido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\ColeccionRecursosGespro\contenido\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13332" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="recursos " sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">COLECCION!$A$1:$XEF$106</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'recursos '!$A$1:$XEI$99</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -831,7 +831,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1540,7 +1540,7 @@
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="6"/>
     <col min="2" max="2" width="22" style="5"/>
@@ -1552,7 +1552,7 @@
     <col min="9" max="16384" width="22" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16363" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16363" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>171</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:16363" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16363" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>181</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16363" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16363" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>176</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16363" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16363" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>174</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16363" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16363" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>180</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16363" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16363" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>174</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16363" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16363" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>176</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16363" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16363" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>176</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16363" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16363" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>172</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16363" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16363" s="8" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>178</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16363" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16363" s="8" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>178</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16363" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16363" s="8" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>178</v>
       </c>
@@ -18216,7 +18216,7 @@
       <c r="XEH12" s="7"/>
       <c r="XEI12" s="7"/>
     </row>
-    <row r="13" spans="1:16363" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16363" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>178</v>
       </c>
@@ -18242,7 +18242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16363" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16363" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>176</v>
       </c>
@@ -18268,7 +18268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16363" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16363" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>176</v>
       </c>
@@ -18294,7 +18294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16363" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16363" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>189</v>
       </c>
@@ -18320,7 +18320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>173</v>
       </c>
@@ -18346,7 +18346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>173</v>
       </c>
@@ -18372,7 +18372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>173</v>
       </c>
@@ -18398,7 +18398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>173</v>
       </c>
@@ -18424,7 +18424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>188</v>
       </c>
@@ -18450,7 +18450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>188</v>
       </c>
@@ -18476,7 +18476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>188</v>
       </c>
@@ -18502,7 +18502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>177</v>
       </c>
@@ -18528,7 +18528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>177</v>
       </c>
@@ -18554,7 +18554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>174</v>
       </c>
@@ -18580,7 +18580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>173</v>
       </c>
@@ -18606,7 +18606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>188</v>
       </c>
@@ -18632,7 +18632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>188</v>
       </c>
@@ -18658,7 +18658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>173</v>
       </c>
@@ -18684,7 +18684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>188</v>
       </c>
@@ -18710,7 +18710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>173</v>
       </c>
@@ -18736,7 +18736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>180</v>
       </c>
@@ -18762,7 +18762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>180</v>
       </c>
@@ -18788,7 +18788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>181</v>
       </c>
@@ -18814,7 +18814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>179</v>
       </c>
@@ -18840,7 +18840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>180</v>
       </c>
@@ -18866,7 +18866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>177</v>
       </c>
@@ -18892,7 +18892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>188</v>
       </c>
@@ -18918,7 +18918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>181</v>
       </c>
@@ -18944,7 +18944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>181</v>
       </c>
@@ -18970,7 +18970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>181</v>
       </c>
@@ -18996,7 +18996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>172</v>
       </c>
@@ -19022,7 +19022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>173</v>
       </c>
@@ -19048,7 +19048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>172</v>
       </c>
@@ -19074,7 +19074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>176</v>
       </c>
@@ -19100,7 +19100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>175</v>
       </c>
@@ -19126,7 +19126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>174</v>
       </c>
@@ -19152,7 +19152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>181</v>
       </c>
@@ -19178,7 +19178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>178</v>
       </c>
@@ -19204,7 +19204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>178</v>
       </c>
@@ -19230,7 +19230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>173</v>
       </c>
@@ -19256,7 +19256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>176</v>
       </c>
@@ -19282,7 +19282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>187</v>
       </c>
@@ -19308,7 +19308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>187</v>
       </c>
@@ -19334,7 +19334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>187</v>
       </c>
@@ -19360,7 +19360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>187</v>
       </c>
@@ -19386,7 +19386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>173</v>
       </c>
@@ -19412,7 +19412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>173</v>
       </c>
@@ -19438,7 +19438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>173</v>
       </c>
@@ -19464,7 +19464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>173</v>
       </c>
@@ -19490,7 +19490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>188</v>
       </c>
@@ -19516,7 +19516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>188</v>
       </c>
@@ -19542,7 +19542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>188</v>
       </c>
@@ -19568,7 +19568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>178</v>
       </c>
@@ -19594,7 +19594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>174</v>
       </c>
@@ -19620,7 +19620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>180</v>
       </c>
@@ -19646,7 +19646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>174</v>
       </c>
@@ -19672,7 +19672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>176</v>
       </c>
@@ -19698,7 +19698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>174</v>
       </c>
@@ -19724,7 +19724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>174</v>
       </c>
@@ -19750,7 +19750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>172</v>
       </c>
@@ -19776,7 +19776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>176</v>
       </c>
@@ -19802,7 +19802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>176</v>
       </c>
@@ -19828,7 +19828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>172</v>
       </c>
@@ -19854,7 +19854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>181</v>
       </c>
@@ -19880,7 +19880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>178</v>
       </c>
@@ -19906,7 +19906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>174</v>
       </c>
@@ -19932,7 +19932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>176</v>
       </c>
@@ -19958,7 +19958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>181</v>
       </c>
@@ -19984,7 +19984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>28</v>
       </c>
@@ -20010,7 +20010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="21" t="s">
         <v>190</v>
       </c>
@@ -20036,7 +20036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>181</v>
       </c>
@@ -20062,7 +20062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>173</v>
       </c>
@@ -20088,7 +20088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>173</v>
       </c>
@@ -20114,7 +20114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>173</v>
       </c>
@@ -20140,7 +20140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>173</v>
       </c>
@@ -20166,7 +20166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>188</v>
       </c>
@@ -20192,7 +20192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>173</v>
       </c>
@@ -20218,7 +20218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>173</v>
       </c>
@@ -20244,7 +20244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>173</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="23" t="s">
         <v>174</v>
       </c>
@@ -20296,7 +20296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>178</v>
       </c>
@@ -20322,7 +20322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
         <v>28</v>
       </c>
@@ -20348,7 +20348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>28</v>
       </c>
@@ -20374,7 +20374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>28</v>
       </c>
@@ -20400,7 +20400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>174</v>
       </c>
@@ -20426,7 +20426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>28</v>
       </c>
@@ -20452,7 +20452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>181</v>
       </c>
@@ -20478,7 +20478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="18" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" s="18" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="19"/>
       <c r="B100" s="19"/>
       <c r="C100" s="19"/>
@@ -20486,7 +20486,7 @@
       <c r="E100" s="19"/>
       <c r="F100" s="19"/>
     </row>
-    <row r="104" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D104" s="26"/>
     </row>
   </sheetData>
@@ -20599,22 +20599,22 @@
   <dimension ref="A1:XEF117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="24"/>
-    <col min="2" max="2" width="17.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="12" customWidth="1"/>
     <col min="4" max="4" width="22" style="24"/>
-    <col min="5" max="5" width="5.6640625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="32" customWidth="1"/>
     <col min="6" max="16384" width="22" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16360" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16360" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>171</v>
       </c>
@@ -20629,7 +20629,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:16360" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16360" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>222</v>
       </c>
@@ -20638,7 +20638,7 @@
       <c r="D2" s="50"/>
       <c r="E2" s="51"/>
     </row>
-    <row r="3" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16360" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>181</v>
       </c>
@@ -20655,7 +20655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16360" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>176</v>
       </c>
@@ -20672,7 +20672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16360" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>174</v>
       </c>
@@ -20689,7 +20689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16360" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>180</v>
       </c>
@@ -20706,7 +20706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16360" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>174</v>
       </c>
@@ -20723,7 +20723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16360" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>176</v>
       </c>
@@ -20740,7 +20740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16360" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>176</v>
       </c>
@@ -20757,7 +20757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16360" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>172</v>
       </c>
@@ -20774,7 +20774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16360" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16360" s="8" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
         <v>178</v>
       </c>
@@ -20791,7 +20791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16360" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16360" s="8" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
         <v>178</v>
       </c>
@@ -20808,7 +20808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16360" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16360" s="8" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
         <v>178</v>
       </c>
@@ -37180,7 +37180,7 @@
       <c r="XEE13" s="7"/>
       <c r="XEF13" s="7"/>
     </row>
-    <row r="14" spans="1:16360" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16360" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
         <v>178</v>
       </c>
@@ -37197,7 +37197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16360" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16360" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
         <v>176</v>
       </c>
@@ -37214,7 +37214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16360" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16360" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="s">
         <v>176</v>
       </c>
@@ -37231,7 +37231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="41" t="s">
         <v>189</v>
       </c>
@@ -37248,7 +37248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="41" t="s">
         <v>173</v>
       </c>
@@ -37265,7 +37265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
         <v>173</v>
       </c>
@@ -37282,7 +37282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
         <v>173</v>
       </c>
@@ -37299,7 +37299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
         <v>173</v>
       </c>
@@ -37316,7 +37316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
         <v>188</v>
       </c>
@@ -37333,7 +37333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
         <v>188</v>
       </c>
@@ -37350,7 +37350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
         <v>188</v>
       </c>
@@ -37367,7 +37367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
         <v>177</v>
       </c>
@@ -37384,7 +37384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
         <v>177</v>
       </c>
@@ -37401,7 +37401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
         <v>174</v>
       </c>
@@ -37418,7 +37418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>173</v>
       </c>
@@ -37435,7 +37435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
         <v>188</v>
       </c>
@@ -37452,7 +37452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
         <v>188</v>
       </c>
@@ -37469,7 +37469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
         <v>173</v>
       </c>
@@ -37486,7 +37486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
         <v>188</v>
       </c>
@@ -37503,7 +37503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="41" t="s">
         <v>173</v>
       </c>
@@ -37520,7 +37520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="41" t="s">
         <v>180</v>
       </c>
@@ -37537,7 +37537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
         <v>180</v>
       </c>
@@ -37554,7 +37554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="s">
         <v>181</v>
       </c>
@@ -37571,7 +37571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="41" t="s">
         <v>218</v>
       </c>
@@ -37588,7 +37588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="41" t="s">
         <v>180</v>
       </c>
@@ -37605,7 +37605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="36" t="s">
         <v>177</v>
       </c>
@@ -37622,7 +37622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="36" t="s">
         <v>188</v>
       </c>
@@ -37639,7 +37639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="36" t="s">
         <v>181</v>
       </c>
@@ -37656,7 +37656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>181</v>
       </c>
@@ -37673,7 +37673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>181</v>
       </c>
@@ -37690,7 +37690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
         <v>172</v>
       </c>
@@ -37707,7 +37707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="41" t="s">
         <v>173</v>
       </c>
@@ -37724,7 +37724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
         <v>172</v>
       </c>
@@ -37741,7 +37741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="41" t="s">
         <v>176</v>
       </c>
@@ -37758,7 +37758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="41" t="s">
         <v>175</v>
       </c>
@@ -37775,7 +37775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="41" t="s">
         <v>174</v>
       </c>
@@ -37792,7 +37792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
         <v>181</v>
       </c>
@@ -37809,7 +37809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="41" t="s">
         <v>178</v>
       </c>
@@ -37826,7 +37826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="46" t="s">
         <v>178</v>
       </c>
@@ -37843,7 +37843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="41" t="s">
         <v>173</v>
       </c>
@@ -37860,7 +37860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="41" t="s">
         <v>176</v>
       </c>
@@ -37877,7 +37877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="41" t="s">
         <v>219</v>
       </c>
@@ -37894,7 +37894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="41" t="s">
         <v>219</v>
       </c>
@@ -37911,7 +37911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="41" t="s">
         <v>219</v>
       </c>
@@ -37928,7 +37928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="41" t="s">
         <v>219</v>
       </c>
@@ -37945,7 +37945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="41" t="s">
         <v>173</v>
       </c>
@@ -37962,7 +37962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="41" t="s">
         <v>173</v>
       </c>
@@ -37979,7 +37979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="41" t="s">
         <v>173</v>
       </c>
@@ -37996,7 +37996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="41" t="s">
         <v>173</v>
       </c>
@@ -38013,7 +38013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="41" t="s">
         <v>188</v>
       </c>
@@ -38030,7 +38030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="41" t="s">
         <v>188</v>
       </c>
@@ -38047,7 +38047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="41" t="s">
         <v>188</v>
       </c>
@@ -38064,7 +38064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="41" t="s">
         <v>178</v>
       </c>
@@ -38081,7 +38081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="41" t="s">
         <v>174</v>
       </c>
@@ -38098,7 +38098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="41" t="s">
         <v>180</v>
       </c>
@@ -38115,7 +38115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="41" t="s">
         <v>174</v>
       </c>
@@ -38132,7 +38132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="41" t="s">
         <v>176</v>
       </c>
@@ -38149,7 +38149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="41" t="s">
         <v>174</v>
       </c>
@@ -38166,7 +38166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="41" t="s">
         <v>174</v>
       </c>
@@ -38183,7 +38183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="41" t="s">
         <v>172</v>
       </c>
@@ -38200,7 +38200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="41" t="s">
         <v>176</v>
       </c>
@@ -38217,7 +38217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="41" t="s">
         <v>176</v>
       </c>
@@ -38234,7 +38234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="41" t="s">
         <v>172</v>
       </c>
@@ -38251,7 +38251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="41" t="s">
         <v>181</v>
       </c>
@@ -38268,7 +38268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="41" t="s">
         <v>178</v>
       </c>
@@ -38285,7 +38285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="41" t="s">
         <v>174</v>
       </c>
@@ -38302,7 +38302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="41" t="s">
         <v>176</v>
       </c>
@@ -38319,7 +38319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="41" t="s">
         <v>181</v>
       </c>
@@ -38336,7 +38336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="41" t="s">
         <v>28</v>
       </c>
@@ -38353,7 +38353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="41" t="s">
         <v>190</v>
       </c>
@@ -38370,7 +38370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="41" t="s">
         <v>181</v>
       </c>
@@ -38387,7 +38387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="41" t="s">
         <v>173</v>
       </c>
@@ -38404,7 +38404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="41" t="s">
         <v>173</v>
       </c>
@@ -38421,7 +38421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="41" t="s">
         <v>173</v>
       </c>
@@ -38438,7 +38438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="41" t="s">
         <v>173</v>
       </c>
@@ -38455,7 +38455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="41" t="s">
         <v>188</v>
       </c>
@@ -38472,7 +38472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="41" t="s">
         <v>173</v>
       </c>
@@ -38489,7 +38489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="41" t="s">
         <v>173</v>
       </c>
@@ -38506,7 +38506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="41" t="s">
         <v>173</v>
       </c>
@@ -38523,7 +38523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="41" t="s">
         <v>174</v>
       </c>
@@ -38540,7 +38540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="41" t="s">
         <v>178</v>
       </c>
@@ -38557,7 +38557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="36" t="s">
         <v>28</v>
       </c>
@@ -38574,7 +38574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="41" t="s">
         <v>28</v>
       </c>
@@ -38591,7 +38591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="41" t="s">
         <v>28</v>
       </c>
@@ -38608,7 +38608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="41" t="s">
         <v>174</v>
       </c>
@@ -38625,7 +38625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="36" t="s">
         <v>28</v>
       </c>
@@ -38642,7 +38642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="36" t="s">
         <v>181</v>
       </c>
@@ -38659,7 +38659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="36" t="s">
         <v>221</v>
       </c>
@@ -38676,7 +38676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="36" t="s">
         <v>178</v>
       </c>
@@ -38696,7 +38696,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="103" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="36" t="s">
         <v>181</v>
       </c>
@@ -38713,7 +38713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="41" t="s">
         <v>218</v>
       </c>
@@ -38730,7 +38730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="36" t="s">
         <v>213</v>
       </c>
@@ -38747,7 +38747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="41" t="s">
         <v>178</v>
       </c>
@@ -38764,41 +38764,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11"/>
       <c r="B107" s="31"/>
       <c r="C107" s="16"/>
       <c r="D107" s="11"/>
       <c r="E107" s="33"/>
     </row>
-    <row r="108" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="11"/>
       <c r="B108" s="10"/>
       <c r="C108" s="16"/>
       <c r="D108" s="11"/>
       <c r="E108" s="33"/>
     </row>
-    <row r="109" spans="1:6" s="9" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" s="9" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11"/>
       <c r="B109" s="10"/>
       <c r="C109" s="16"/>
       <c r="D109" s="11"/>
       <c r="E109" s="33"/>
     </row>
-    <row r="110" spans="1:6" s="18" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" s="18" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="19"/>
       <c r="B110" s="19"/>
       <c r="C110" s="19"/>
       <c r="D110" s="19"/>
       <c r="E110" s="34"/>
     </row>
-    <row r="111" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E111" s="32">
         <f>SUBTOTAL(9,E3:E110)</f>
         <v>104</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="27" t="s">
         <v>205</v>
       </c>
@@ -38806,7 +38806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="27" t="s">
         <v>206</v>
       </c>
@@ -38814,7 +38814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="27" t="s">
         <v>207</v>
       </c>
@@ -38822,7 +38822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="27" t="s">
         <v>203</v>
       </c>
@@ -38830,7 +38830,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="27" t="s">
         <v>204</v>
       </c>
@@ -38838,7 +38838,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="29" t="s">
         <v>208</v>
       </c>

</xml_diff>